<commit_message>
add slices for the extra codes MHV/PGHD has historically used
</commit_message>
<xml_diff>
--- a/docs/observations-summary.xlsx
+++ b/docs/observations-summary.xlsx
@@ -59,7 +59,7 @@
     <t/>
   </si>
   <si>
-    <t>null#2708-6</t>
+    <t>null#2708-6, null#59408-5</t>
   </si>
   <si>
     <t>http://hl7.org/fhir/ValueSet/observation-vitalsignresult (extensible)</t>
@@ -80,7 +80,7 @@
     <t>VA MHV Blood Pressure Observation</t>
   </si>
   <si>
-    <t>null#85354-9</t>
+    <t>null#85354-9, null#55284-4, null#8716-3</t>
   </si>
   <si>
     <t>optional</t>

</xml_diff>